<commit_message>
correct version of .xlsx and added pylab.show() to 161017_loadBelarus
</commit_message>
<xml_diff>
--- a/diary/Belarus-cascade-data.xlsx
+++ b/diary/Belarus-cascade-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="260" yWindow="-23540" windowWidth="25600" windowHeight="23540" activeTab="3"/>
+    <workbookView xWindow="260" yWindow="-23540" windowWidth="25600" windowHeight="14520" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="103">
   <si>
     <t>Name</t>
   </si>
@@ -341,9 +341,6 @@
   <si>
     <t>y</t>
   </si>
-  <si>
-    <t>Susceptible (non infected, non vaccinated)</t>
-  </si>
 </sst>
 </file>
 
@@ -427,13 +424,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -2810,10 +2806,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI69"/>
+  <dimension ref="A1:AI62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:U13"/>
+      <selection activeCell="A10" sqref="A10:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2824,7 +2820,7 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -2926,424 +2922,291 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>97</v>
+    <row r="2" spans="1:35" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>'Population Definitions'!A2</f>
+        <v>0-4</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="str">
-        <f>IF(SUMPRODUCT(--(E2:AI2&lt;&gt;""))=0,0,"N.A.")</f>
+        <f>IF(SUMPRODUCT(--(E2:AI2&lt;&gt;""))=0,1000000,"N.A.")</f>
         <v>N.A.</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3">
-        <f t="shared" ref="E2:G2" si="0">E9-E65-E44</f>
+      <c r="E2" s="2">
         <v>460895</v>
       </c>
-      <c r="F2" s="3">
-        <f t="shared" si="0"/>
+      <c r="F2" s="2">
         <v>454919</v>
       </c>
-      <c r="G2" s="3">
-        <f t="shared" si="0"/>
+      <c r="G2" s="2">
         <v>449853</v>
       </c>
-      <c r="H2" s="3">
-        <f>H9-H65-H44</f>
-        <v>445863.89238974912</v>
-      </c>
-      <c r="I2" s="3">
-        <f t="shared" ref="I2:U2" si="1">I9-I65-I44</f>
-        <v>445102.60250410484</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" si="1"/>
-        <v>449288.02092334506</v>
-      </c>
-      <c r="K2" s="3">
-        <f t="shared" si="1"/>
-        <v>462374.10295544215</v>
-      </c>
-      <c r="L2" s="3">
-        <f t="shared" si="1"/>
-        <v>472709.88233686809</v>
-      </c>
-      <c r="M2" s="3">
-        <f t="shared" si="1"/>
-        <v>482485.35912951664</v>
-      </c>
-      <c r="N2" s="3">
-        <f t="shared" si="1"/>
-        <v>494089.29217810772</v>
-      </c>
-      <c r="O2" s="3">
-        <f t="shared" si="1"/>
-        <v>509307.39879470621</v>
-      </c>
-      <c r="P2" s="3">
-        <f t="shared" si="1"/>
-        <v>526554.66045744589</v>
-      </c>
-      <c r="Q2" s="3">
-        <f t="shared" si="1"/>
-        <v>545880.06667153363</v>
-      </c>
-      <c r="R2" s="3">
-        <f t="shared" si="1"/>
-        <v>564855.90276820015</v>
-      </c>
-      <c r="S2" s="3">
-        <f t="shared" si="1"/>
-        <v>579051.60993921349</v>
-      </c>
-      <c r="T2" s="3">
-        <f t="shared" si="1"/>
-        <v>586267.25645906897</v>
-      </c>
-      <c r="U2" s="3">
-        <f t="shared" si="1"/>
+      <c r="H2" s="2">
+        <v>445935</v>
+      </c>
+      <c r="I2" s="2">
+        <v>445183</v>
+      </c>
+      <c r="J2" s="2">
+        <v>449370</v>
+      </c>
+      <c r="K2" s="2">
+        <v>462460</v>
+      </c>
+      <c r="L2" s="2">
+        <v>472794</v>
+      </c>
+      <c r="M2" s="2">
+        <v>482564</v>
+      </c>
+      <c r="N2" s="2">
+        <v>494176</v>
+      </c>
+      <c r="O2" s="2">
+        <v>509391</v>
+      </c>
+      <c r="P2" s="2">
+        <v>526635</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>545959</v>
+      </c>
+      <c r="R2" s="2">
+        <v>564931</v>
+      </c>
+      <c r="S2" s="2">
+        <v>579119</v>
+      </c>
+      <c r="T2" s="2">
+        <v>586330</v>
+      </c>
+      <c r="U2" s="2">
         <v>597926</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>98</v>
+      <c r="A3" t="str">
+        <f>'Population Definitions'!A3</f>
+        <v>5-14</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(SUMPRODUCT(--(E3:AI3&lt;&gt;""))=0,0,"N.A.")</f>
+        <f>IF(SUMPRODUCT(--(E3:AI3&lt;&gt;""))=0,1000000,"N.A.")</f>
         <v>N.A.</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3">
-        <f t="shared" ref="E3:U3" si="2">E10-E66-E45</f>
+      <c r="E3">
         <v>1378121</v>
       </c>
-      <c r="F3" s="3">
-        <f t="shared" si="2"/>
+      <c r="F3">
         <v>1311002</v>
       </c>
-      <c r="G3" s="3">
-        <f t="shared" si="2"/>
+      <c r="G3">
         <v>1241841</v>
       </c>
-      <c r="H3" s="3">
-        <f t="shared" si="2"/>
-        <v>1173884.6666666667</v>
-      </c>
-      <c r="I3" s="3">
-        <f t="shared" si="2"/>
-        <v>1111432.8333333333</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" si="2"/>
-        <v>1055946.3333333335</v>
-      </c>
-      <c r="K3" s="3">
-        <f t="shared" si="2"/>
-        <v>1006470.1111111111</v>
-      </c>
-      <c r="L3" s="3">
-        <f t="shared" si="2"/>
-        <v>966454.88888888888</v>
-      </c>
-      <c r="M3" s="3">
-        <f t="shared" si="2"/>
-        <v>936053.77777777775</v>
-      </c>
-      <c r="N3" s="3">
-        <f t="shared" si="2"/>
-        <v>914259.83333333337</v>
-      </c>
-      <c r="O3" s="3">
-        <f t="shared" si="2"/>
-        <v>899577.72222222225</v>
-      </c>
-      <c r="P3" s="3">
-        <f t="shared" si="2"/>
-        <v>889054</v>
-      </c>
-      <c r="Q3" s="3">
-        <f t="shared" si="2"/>
-        <v>889819.38888888888</v>
-      </c>
-      <c r="R3" s="3">
-        <f t="shared" si="2"/>
-        <v>900957.11111111112</v>
-      </c>
-      <c r="S3" s="3">
-        <f t="shared" si="2"/>
-        <v>918846.66666666663</v>
-      </c>
-      <c r="T3" s="3">
-        <f t="shared" si="2"/>
-        <v>939315.72222222225</v>
-      </c>
-      <c r="U3" s="3">
-        <f t="shared" si="2"/>
+      <c r="H3">
+        <v>1174143</v>
+      </c>
+      <c r="I3">
+        <v>1111714</v>
+      </c>
+      <c r="J3">
+        <v>1056221</v>
+      </c>
+      <c r="K3">
+        <v>1006743</v>
+      </c>
+      <c r="L3">
+        <v>966711</v>
+      </c>
+      <c r="M3">
+        <v>936285</v>
+      </c>
+      <c r="N3">
+        <v>914507</v>
+      </c>
+      <c r="O3">
+        <v>899809</v>
+      </c>
+      <c r="P3">
+        <v>889270</v>
+      </c>
+      <c r="Q3">
+        <v>890027</v>
+      </c>
+      <c r="R3">
+        <v>901152</v>
+      </c>
+      <c r="S3">
+        <v>919021</v>
+      </c>
+      <c r="T3">
+        <v>939479</v>
+      </c>
+      <c r="U3">
         <v>964853</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>101</v>
+      <c r="A4" t="str">
+        <f>'Population Definitions'!A4</f>
+        <v>15-64</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="str">
-        <f>IF(SUMPRODUCT(--(E4:AI4&lt;&gt;""))=0,0,"N.A.")</f>
+        <f>IF(SUMPRODUCT(--(E4:AI4&lt;&gt;""))=0,1000000,"N.A.")</f>
         <v>N.A.</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3">
-        <f t="shared" ref="E4:U4" si="3">E11-E67-E46</f>
+      <c r="E4">
         <v>8083506.9999999991</v>
       </c>
-      <c r="F4" s="3">
-        <f t="shared" si="3"/>
+      <c r="F4">
         <v>8096108.9999999991</v>
       </c>
-      <c r="G4" s="3">
-        <f t="shared" si="3"/>
+      <c r="G4">
         <v>8104618.0000000009</v>
       </c>
-      <c r="H4" s="3">
-        <f t="shared" si="3"/>
-        <v>8104020.2257230803</v>
-      </c>
-      <c r="I4" s="3">
-        <f t="shared" si="3"/>
-        <v>8103713.2691707723</v>
-      </c>
-      <c r="J4" s="3">
-        <f t="shared" si="3"/>
-        <v>8099977.6875900123</v>
-      </c>
-      <c r="K4" s="3">
-        <f t="shared" si="3"/>
-        <v>8090019.3251776639</v>
-      </c>
-      <c r="L4" s="3">
-        <f t="shared" si="3"/>
-        <v>8081886.660114646</v>
-      </c>
-      <c r="M4" s="3">
-        <f t="shared" si="3"/>
-        <v>8073441.9146850724</v>
-      </c>
-      <c r="N4" s="3">
-        <f t="shared" si="3"/>
-        <v>8062149.9588447753</v>
-      </c>
-      <c r="O4" s="3">
-        <f t="shared" si="3"/>
-        <v>8048760.84323915</v>
-      </c>
-      <c r="P4" s="3">
-        <f t="shared" si="3"/>
-        <v>8037920.6604574462</v>
-      </c>
-      <c r="Q4" s="3">
-        <f t="shared" si="3"/>
-        <v>8021300.8444493124</v>
-      </c>
-      <c r="R4" s="3">
-        <f t="shared" si="3"/>
-        <v>7997798.1249904223</v>
-      </c>
-      <c r="S4" s="3">
-        <f t="shared" si="3"/>
-        <v>7969293.9432725478</v>
-      </c>
-      <c r="T4" s="3">
-        <f t="shared" si="3"/>
-        <v>7937688.7009035107</v>
-      </c>
-      <c r="U4" s="3">
-        <f t="shared" si="3"/>
+      <c r="H4">
+        <v>8109257.9999999981</v>
+      </c>
+      <c r="I4">
+        <v>8109417</v>
+      </c>
+      <c r="J4">
+        <v>8105553</v>
+      </c>
+      <c r="K4">
+        <v>8095563</v>
+      </c>
+      <c r="L4">
+        <v>8087093</v>
+      </c>
+      <c r="M4">
+        <v>8078145</v>
+      </c>
+      <c r="N4">
+        <v>8067180.0000000009</v>
+      </c>
+      <c r="O4">
+        <v>8053470</v>
+      </c>
+      <c r="P4">
+        <v>8042321</v>
+      </c>
+      <c r="Q4">
+        <v>8025532.0000000009</v>
+      </c>
+      <c r="R4">
+        <v>8001771</v>
+      </c>
+      <c r="S4">
+        <v>7972848.0000000009</v>
+      </c>
+      <c r="T4">
+        <v>7941016.9999999981</v>
+      </c>
+      <c r="U4">
         <v>7889742.0000000009</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>99</v>
+      <c r="A5" t="str">
+        <f>'Population Definitions'!A5</f>
+        <v>65+</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="str">
-        <f>IF(SUMPRODUCT(--(E5:AI5&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
+      <c r="C5">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
-        <f t="shared" ref="E5:U5" si="4">E12-E68-E47</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>100</v>
+      <c r="A6" t="str">
+        <f>'Population Definitions'!A6</f>
+        <v>Prisoners</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="str">
-        <f>IF(SUMPRODUCT(--(E6:AI6&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
+      <c r="C6">
+        <v>29000</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3">
-        <f t="shared" ref="E6:U6" si="5">E13-E69-E48</f>
+      <c r="E6">
         <v>29000</v>
       </c>
-      <c r="F6" s="3">
-        <f t="shared" si="5"/>
+      <c r="F6">
         <v>29000</v>
       </c>
-      <c r="G6" s="3">
-        <f t="shared" si="5"/>
+      <c r="G6">
         <v>29000</v>
       </c>
-      <c r="H6" s="3">
-        <f t="shared" si="5"/>
-        <v>28472.225723082469</v>
-      </c>
-      <c r="I6" s="3">
-        <f t="shared" si="5"/>
-        <v>28506.26917077152</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" si="5"/>
-        <v>28513.576478900606</v>
-      </c>
-      <c r="K6" s="3">
-        <f t="shared" si="5"/>
-        <v>28658.547399886575</v>
-      </c>
-      <c r="L6" s="3">
-        <f t="shared" si="5"/>
-        <v>28624.771225757002</v>
-      </c>
-      <c r="M6" s="3">
-        <f t="shared" si="5"/>
-        <v>28651.359129516641</v>
-      </c>
-      <c r="N6" s="3">
-        <f t="shared" si="5"/>
-        <v>28731.069955885509</v>
-      </c>
-      <c r="O6" s="3">
-        <f t="shared" si="5"/>
-        <v>28748.621016928439</v>
-      </c>
-      <c r="P6" s="3">
-        <f t="shared" si="5"/>
-        <v>28765.2160130015</v>
-      </c>
-      <c r="Q6" s="3">
-        <f t="shared" si="5"/>
-        <v>28744.400004866962</v>
-      </c>
-      <c r="R6" s="3">
-        <f t="shared" si="5"/>
-        <v>28807.124990422326</v>
-      </c>
-      <c r="S6" s="3">
-        <f t="shared" si="5"/>
-        <v>28815.943272546847</v>
-      </c>
-      <c r="T6" s="3">
-        <f t="shared" si="5"/>
-        <v>28845.034236846739</v>
-      </c>
-      <c r="U6" s="3">
-        <f t="shared" si="5"/>
+      <c r="H6">
+        <v>29000</v>
+      </c>
+      <c r="I6">
+        <v>29000</v>
+      </c>
+      <c r="J6">
+        <v>29000</v>
+      </c>
+      <c r="K6">
+        <v>29000</v>
+      </c>
+      <c r="L6">
+        <v>29000</v>
+      </c>
+      <c r="M6">
+        <v>29000</v>
+      </c>
+      <c r="N6">
+        <v>29000</v>
+      </c>
+      <c r="O6">
+        <v>29000</v>
+      </c>
+      <c r="P6">
+        <v>29000</v>
+      </c>
+      <c r="Q6">
+        <v>29000</v>
+      </c>
+      <c r="R6">
+        <v>29000</v>
+      </c>
+      <c r="S6">
+        <v>29000</v>
+      </c>
+      <c r="T6">
+        <v>29000</v>
+      </c>
+      <c r="U6">
         <v>29000</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -3445,71 +3308,19 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>'Population Definitions'!A2</f>
         <v>0-4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="str">
-        <f>IF(SUMPRODUCT(--(E9:AI9&lt;&gt;""))=0,1000000,"N.A.")</f>
-        <v>N.A.</v>
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" s="2">
-        <v>460895</v>
-      </c>
-      <c r="F9" s="2">
-        <v>454919</v>
-      </c>
-      <c r="G9" s="2">
-        <v>449853</v>
-      </c>
-      <c r="H9" s="2">
-        <v>445935</v>
-      </c>
-      <c r="I9" s="2">
-        <v>445183</v>
-      </c>
-      <c r="J9" s="2">
-        <v>449370</v>
-      </c>
-      <c r="K9" s="2">
-        <v>462460</v>
-      </c>
-      <c r="L9" s="2">
-        <v>472794</v>
-      </c>
-      <c r="M9" s="2">
-        <v>482564</v>
-      </c>
-      <c r="N9" s="2">
-        <v>494176</v>
-      </c>
-      <c r="O9" s="2">
-        <v>509391</v>
-      </c>
-      <c r="P9" s="2">
-        <v>526635</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>545959</v>
-      </c>
-      <c r="R9" s="2">
-        <v>564931</v>
-      </c>
-      <c r="S9" s="2">
-        <v>579119</v>
-      </c>
-      <c r="T9" s="2">
-        <v>586330</v>
-      </c>
-      <c r="U9" s="2">
-        <v>597926</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
@@ -3518,65 +3329,13 @@
         <v>5-14</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="str">
-        <f>IF(SUMPRODUCT(--(E10:AI10&lt;&gt;""))=0,1000000,"N.A.")</f>
-        <v>N.A.</v>
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.01</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
-      </c>
-      <c r="E10">
-        <v>1378121</v>
-      </c>
-      <c r="F10">
-        <v>1311002</v>
-      </c>
-      <c r="G10">
-        <v>1241841</v>
-      </c>
-      <c r="H10">
-        <v>1174143</v>
-      </c>
-      <c r="I10">
-        <v>1111714</v>
-      </c>
-      <c r="J10">
-        <v>1056221</v>
-      </c>
-      <c r="K10">
-        <v>1006743</v>
-      </c>
-      <c r="L10">
-        <v>966711</v>
-      </c>
-      <c r="M10">
-        <v>936285</v>
-      </c>
-      <c r="N10">
-        <v>914507</v>
-      </c>
-      <c r="O10">
-        <v>899809</v>
-      </c>
-      <c r="P10">
-        <v>889270</v>
-      </c>
-      <c r="Q10">
-        <v>890027</v>
-      </c>
-      <c r="R10">
-        <v>901152</v>
-      </c>
-      <c r="S10">
-        <v>919021</v>
-      </c>
-      <c r="T10">
-        <v>939479</v>
-      </c>
-      <c r="U10">
-        <v>964853</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -3585,65 +3344,13 @@
         <v>15-64</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="str">
-        <f>IF(SUMPRODUCT(--(E11:AI11&lt;&gt;""))=0,1000000,"N.A.")</f>
-        <v>N.A.</v>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.01</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
-      </c>
-      <c r="E11">
-        <v>8083506.9999999991</v>
-      </c>
-      <c r="F11">
-        <v>8096108.9999999991</v>
-      </c>
-      <c r="G11">
-        <v>8104618.0000000009</v>
-      </c>
-      <c r="H11">
-        <v>8109257.9999999981</v>
-      </c>
-      <c r="I11">
-        <v>8109417</v>
-      </c>
-      <c r="J11">
-        <v>8105553</v>
-      </c>
-      <c r="K11">
-        <v>8095563</v>
-      </c>
-      <c r="L11">
-        <v>8087093</v>
-      </c>
-      <c r="M11">
-        <v>8078145</v>
-      </c>
-      <c r="N11">
-        <v>8067180.0000000009</v>
-      </c>
-      <c r="O11">
-        <v>8053470</v>
-      </c>
-      <c r="P11">
-        <v>8042321</v>
-      </c>
-      <c r="Q11">
-        <v>8025532.0000000009</v>
-      </c>
-      <c r="R11">
-        <v>8001771</v>
-      </c>
-      <c r="S11">
-        <v>7972848.0000000009</v>
-      </c>
-      <c r="T11">
-        <v>7941016.9999999981</v>
-      </c>
-      <c r="U11">
-        <v>7889742.0000000009</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
@@ -3652,10 +3359,10 @@
         <v>65+</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -3667,69 +3374,18 @@
         <v>Prisoners</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>29000</v>
+        <v>0.01</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
-      </c>
-      <c r="E13">
-        <v>29000</v>
-      </c>
-      <c r="F13">
-        <v>29000</v>
-      </c>
-      <c r="G13">
-        <v>29000</v>
-      </c>
-      <c r="H13">
-        <v>29000</v>
-      </c>
-      <c r="I13">
-        <v>29000</v>
-      </c>
-      <c r="J13">
-        <v>29000</v>
-      </c>
-      <c r="K13">
-        <v>29000</v>
-      </c>
-      <c r="L13">
-        <v>29000</v>
-      </c>
-      <c r="M13">
-        <v>29000</v>
-      </c>
-      <c r="N13">
-        <v>29000</v>
-      </c>
-      <c r="O13">
-        <v>29000</v>
-      </c>
-      <c r="P13">
-        <v>29000</v>
-      </c>
-      <c r="Q13">
-        <v>29000</v>
-      </c>
-      <c r="R13">
-        <v>29000</v>
-      </c>
-      <c r="S13">
-        <v>29000</v>
-      </c>
-      <c r="T13">
-        <v>29000</v>
-      </c>
-      <c r="U13">
-        <v>29000</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -3840,7 +3496,8 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>0.01</v>
+        <f>IF(SUMPRODUCT(--(E16:AI16&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -3855,7 +3512,8 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>0.01</v>
+        <f>IF(SUMPRODUCT(--(E17:AI17&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -3870,7 +3528,8 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>0.01</v>
+        <f>IF(SUMPRODUCT(--(E18:AI18&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -3885,7 +3544,8 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>0.01</v>
+        <f>IF(SUMPRODUCT(--(E19:AI19&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -3900,7 +3560,8 @@
         <v>10</v>
       </c>
       <c r="C20">
-        <v>0.01</v>
+        <f>IF(SUMPRODUCT(--(E20:AI20&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -3908,7 +3569,7 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -4092,7 +3753,7 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -4202,12 +3863,51 @@
       <c r="B30" t="s">
         <v>10</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="str">
         <f>IF(SUMPRODUCT(--(E30:AI30&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
+      </c>
+      <c r="H30">
+        <v>3.4612500392500412E-4</v>
+      </c>
+      <c r="I30">
+        <v>3.7437566661793217E-4</v>
+      </c>
+      <c r="J30">
+        <v>3.9114059094151154E-4</v>
+      </c>
+      <c r="K30">
+        <v>3.9945210724170614E-4</v>
+      </c>
+      <c r="L30">
+        <v>3.5536495707418308E-4</v>
+      </c>
+      <c r="M30">
+        <v>3.8292505158462383E-4</v>
+      </c>
+      <c r="N30">
+        <v>4.2588577505883409E-4</v>
+      </c>
+      <c r="O30">
+        <v>4.1756643221519692E-4</v>
+      </c>
+      <c r="P30">
+        <v>4.0381955262228705E-4</v>
+      </c>
+      <c r="Q30">
+        <v>3.7399221810413839E-4</v>
+      </c>
+      <c r="R30">
+        <v>3.2803193660007262E-4</v>
+      </c>
+      <c r="S30">
+        <v>2.7763471676790162E-4</v>
+      </c>
+      <c r="T30">
+        <v>1.9575250593329905E-4</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
@@ -4218,12 +3918,51 @@
       <c r="B31" t="s">
         <v>10</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="str">
         <f>IF(SUMPRODUCT(--(E31:AI31&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
+      </c>
+      <c r="H31">
+        <v>3.4612500392500401E-4</v>
+      </c>
+      <c r="I31">
+        <v>3.7437566661793227E-4</v>
+      </c>
+      <c r="J31">
+        <v>3.9114059094151149E-4</v>
+      </c>
+      <c r="K31">
+        <v>3.9945210724170614E-4</v>
+      </c>
+      <c r="L31">
+        <v>3.5536495707418314E-4</v>
+      </c>
+      <c r="M31">
+        <v>3.8292505158462389E-4</v>
+      </c>
+      <c r="N31">
+        <v>4.2588577505883415E-4</v>
+      </c>
+      <c r="O31">
+        <v>4.1756643221519708E-4</v>
+      </c>
+      <c r="P31">
+        <v>4.0381955262228699E-4</v>
+      </c>
+      <c r="Q31">
+        <v>3.7399221810413834E-4</v>
+      </c>
+      <c r="R31">
+        <v>3.2803193660007268E-4</v>
+      </c>
+      <c r="S31">
+        <v>2.7763471676790162E-4</v>
+      </c>
+      <c r="T31">
+        <v>1.9575250593329902E-4</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
@@ -4234,12 +3973,51 @@
       <c r="B32" t="s">
         <v>10</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="str">
         <f>IF(SUMPRODUCT(--(E32:AI32&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
+      </c>
+      <c r="H32">
+        <v>1.3829859750640878E-3</v>
+      </c>
+      <c r="I32">
+        <v>1.4375000132079993E-3</v>
+      </c>
+      <c r="J32">
+        <v>1.4530723652197972E-3</v>
+      </c>
+      <c r="K32">
+        <v>1.4498713290621945E-3</v>
+      </c>
+      <c r="L32">
+        <v>1.265101396838325E-3</v>
+      </c>
+      <c r="M32">
+        <v>1.3451425457596811E-3</v>
+      </c>
+      <c r="N32">
+        <v>1.3765356698801899E-3</v>
+      </c>
+      <c r="O32">
+        <v>1.3602450031543062E-3</v>
+      </c>
+      <c r="P32">
+        <v>1.3194452786842487E-3</v>
+      </c>
+      <c r="Q32">
+        <v>1.2414070227531066E-3</v>
+      </c>
+      <c r="R32">
+        <v>1.128680252675175E-3</v>
+      </c>
+      <c r="S32">
+        <v>9.7815905829049779E-4</v>
+      </c>
+      <c r="T32">
+        <v>6.9432148382400161E-4</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.2">
@@ -4266,17 +4044,38 @@
       <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="str">
         <f>IF(SUMPRODUCT(--(E34:AI34&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
+      </c>
+      <c r="N34">
+        <v>3.0827586206896553E-2</v>
+      </c>
+      <c r="O34">
+        <v>2.8068965517241379E-2</v>
+      </c>
+      <c r="P34">
+        <v>2.8413793103448277E-2</v>
+      </c>
+      <c r="Q34">
+        <v>2.6827586206896552E-2</v>
+      </c>
+      <c r="R34">
+        <v>2.0241379310344827E-2</v>
+      </c>
+      <c r="S34">
+        <v>1.793103448275862E-2</v>
+      </c>
+      <c r="T34">
+        <v>1.5862068965517243E-2</v>
       </c>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -4384,7 +4183,7 @@
         <v>0-4</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" t="str">
         <f>IF(SUMPRODUCT(--(E37:AI37&lt;&gt;""))=0,0,"N.A.")</f>
@@ -4394,43 +4193,43 @@
         <v>12</v>
       </c>
       <c r="H37">
-        <v>3.4612500392500412E-4</v>
+        <v>71.107610250864482</v>
       </c>
       <c r="I37">
-        <v>3.7437566661793217E-4</v>
+        <v>80.397495895146989</v>
       </c>
       <c r="J37">
-        <v>3.9114059094151154E-4</v>
+        <v>81.97907665494813</v>
       </c>
       <c r="K37">
-        <v>3.9945210724170614E-4</v>
+        <v>85.897044557869506</v>
       </c>
       <c r="L37">
-        <v>3.5536495707418308E-4</v>
+        <v>84.117663131886758</v>
       </c>
       <c r="M37">
-        <v>3.8292505158462383E-4</v>
+        <v>78.64087048335972</v>
       </c>
       <c r="N37">
-        <v>4.2588577505883409E-4</v>
+        <v>86.70782189226864</v>
       </c>
       <c r="O37">
-        <v>4.1756643221519692E-4</v>
+        <v>83.601205293783707</v>
       </c>
       <c r="P37">
-        <v>4.0381955262228705E-4</v>
+        <v>80.339542554055541</v>
       </c>
       <c r="Q37">
-        <v>3.7399221810413839E-4</v>
+        <v>78.933328466371606</v>
       </c>
       <c r="R37">
-        <v>3.2803193660007262E-4</v>
+        <v>75.097231799897344</v>
       </c>
       <c r="S37">
-        <v>2.7763471676790162E-4</v>
+        <v>67.390060786486359</v>
       </c>
       <c r="T37">
-        <v>1.9575250593329905E-4</v>
+        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.2">
@@ -4439,7 +4238,7 @@
         <v>5-14</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C38" t="str">
         <f>IF(SUMPRODUCT(--(E38:AI38&lt;&gt;""))=0,0,"N.A.")</f>
@@ -4449,43 +4248,43 @@
         <v>12</v>
       </c>
       <c r="H38">
-        <v>3.4612500392500401E-4</v>
+        <v>71.107610250864482</v>
       </c>
       <c r="I38">
-        <v>3.7437566661793227E-4</v>
+        <v>80.397495895146989</v>
       </c>
       <c r="J38">
-        <v>3.9114059094151149E-4</v>
+        <v>81.97907665494813</v>
       </c>
       <c r="K38">
-        <v>3.9945210724170614E-4</v>
+        <v>85.897044557869506</v>
       </c>
       <c r="L38">
-        <v>3.5536495707418314E-4</v>
+        <v>84.117663131886758</v>
       </c>
       <c r="M38">
-        <v>3.8292505158462389E-4</v>
+        <v>78.64087048335972</v>
       </c>
       <c r="N38">
-        <v>4.2588577505883415E-4</v>
+        <v>86.70782189226864</v>
       </c>
       <c r="O38">
-        <v>4.1756643221519708E-4</v>
+        <v>83.601205293783707</v>
       </c>
       <c r="P38">
-        <v>4.0381955262228699E-4</v>
+        <v>80.339542554055541</v>
       </c>
       <c r="Q38">
-        <v>3.7399221810413834E-4</v>
+        <v>78.933328466371606</v>
       </c>
       <c r="R38">
-        <v>3.2803193660007268E-4</v>
+        <v>75.097231799897344</v>
       </c>
       <c r="S38">
-        <v>2.7763471676790162E-4</v>
+        <v>67.390060786486359</v>
       </c>
       <c r="T38">
-        <v>1.9575250593329902E-4</v>
+        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
@@ -4494,7 +4293,7 @@
         <v>15-64</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" t="str">
         <f>IF(SUMPRODUCT(--(E39:AI39&lt;&gt;""))=0,0,"N.A.")</f>
@@ -4504,43 +4303,43 @@
         <v>12</v>
       </c>
       <c r="H39">
-        <v>1.3829859750640878E-3</v>
+        <v>71.107610250864482</v>
       </c>
       <c r="I39">
-        <v>1.4375000132079993E-3</v>
+        <v>80.397495895146989</v>
       </c>
       <c r="J39">
-        <v>1.4530723652197972E-3</v>
+        <v>81.97907665494813</v>
       </c>
       <c r="K39">
-        <v>1.4498713290621945E-3</v>
+        <v>85.897044557869506</v>
       </c>
       <c r="L39">
-        <v>1.265101396838325E-3</v>
+        <v>84.117663131886758</v>
       </c>
       <c r="M39">
-        <v>1.3451425457596811E-3</v>
+        <v>78.64087048335972</v>
       </c>
       <c r="N39">
-        <v>1.3765356698801899E-3</v>
+        <v>86.70782189226864</v>
       </c>
       <c r="O39">
-        <v>1.3602450031543062E-3</v>
+        <v>83.601205293783707</v>
       </c>
       <c r="P39">
-        <v>1.3194452786842487E-3</v>
+        <v>80.339542554055541</v>
       </c>
       <c r="Q39">
-        <v>1.2414070227531066E-3</v>
+        <v>78.933328466371606</v>
       </c>
       <c r="R39">
-        <v>1.128680252675175E-3</v>
+        <v>75.097231799897344</v>
       </c>
       <c r="S39">
-        <v>9.7815905829049779E-4</v>
+        <v>67.390060786486359</v>
       </c>
       <c r="T39">
-        <v>6.9432148382400161E-4</v>
+        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.2">
@@ -4549,7 +4348,7 @@
         <v>65+</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C40">
         <f>IF(SUMPRODUCT(--(E40:AI40&lt;&gt;""))=0,0,"N.A.")</f>
@@ -4565,7 +4364,7 @@
         <v>Prisoners</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" t="str">
         <f>IF(SUMPRODUCT(--(E41:AI41&lt;&gt;""))=0,0,"N.A.")</f>
@@ -4574,31 +4373,49 @@
       <c r="D41" t="s">
         <v>12</v>
       </c>
+      <c r="H41">
+        <v>71.107610250864482</v>
+      </c>
+      <c r="I41">
+        <v>80.397495895146989</v>
+      </c>
+      <c r="J41">
+        <v>81.97907665494813</v>
+      </c>
+      <c r="K41">
+        <v>85.897044557869506</v>
+      </c>
+      <c r="L41">
+        <v>84.117663131886758</v>
+      </c>
+      <c r="M41">
+        <v>78.64087048335972</v>
+      </c>
       <c r="N41">
-        <v>3.0827586206896553E-2</v>
+        <v>86.70782189226864</v>
       </c>
       <c r="O41">
-        <v>2.8068965517241379E-2</v>
+        <v>83.601205293783707</v>
       </c>
       <c r="P41">
-        <v>2.8413793103448277E-2</v>
+        <v>80.339542554055541</v>
       </c>
       <c r="Q41">
-        <v>2.6827586206896552E-2</v>
+        <v>78.933328466371606</v>
       </c>
       <c r="R41">
-        <v>2.0241379310344827E-2</v>
+        <v>75.097231799897344</v>
       </c>
       <c r="S41">
-        <v>1.793103448275862E-2</v>
+        <v>67.390060786486359</v>
       </c>
       <c r="T41">
-        <v>1.5862068965517243E-2</v>
+        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -4708,51 +4525,12 @@
       <c r="B44" t="s">
         <v>11</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C44">
         <f>IF(SUMPRODUCT(--(E44:AI44&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
-      </c>
-      <c r="H44">
-        <v>71.107610250864482</v>
-      </c>
-      <c r="I44">
-        <v>80.397495895146989</v>
-      </c>
-      <c r="J44">
-        <v>81.97907665494813</v>
-      </c>
-      <c r="K44">
-        <v>85.897044557869506</v>
-      </c>
-      <c r="L44">
-        <v>84.117663131886758</v>
-      </c>
-      <c r="M44">
-        <v>78.64087048335972</v>
-      </c>
-      <c r="N44">
-        <v>86.70782189226864</v>
-      </c>
-      <c r="O44">
-        <v>83.601205293783707</v>
-      </c>
-      <c r="P44">
-        <v>80.339542554055541</v>
-      </c>
-      <c r="Q44">
-        <v>78.933328466371606</v>
-      </c>
-      <c r="R44">
-        <v>75.097231799897344</v>
-      </c>
-      <c r="S44">
-        <v>67.390060786486359</v>
-      </c>
-      <c r="T44">
-        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.2">
@@ -4763,51 +4541,12 @@
       <c r="B45" t="s">
         <v>11</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45">
         <f>IF(SUMPRODUCT(--(E45:AI45&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
-      </c>
-      <c r="H45">
-        <v>71.107610250864482</v>
-      </c>
-      <c r="I45">
-        <v>80.397495895146989</v>
-      </c>
-      <c r="J45">
-        <v>81.97907665494813</v>
-      </c>
-      <c r="K45">
-        <v>85.897044557869506</v>
-      </c>
-      <c r="L45">
-        <v>84.117663131886758</v>
-      </c>
-      <c r="M45">
-        <v>78.64087048335972</v>
-      </c>
-      <c r="N45">
-        <v>86.70782189226864</v>
-      </c>
-      <c r="O45">
-        <v>83.601205293783707</v>
-      </c>
-      <c r="P45">
-        <v>80.339542554055541</v>
-      </c>
-      <c r="Q45">
-        <v>78.933328466371606</v>
-      </c>
-      <c r="R45">
-        <v>75.097231799897344</v>
-      </c>
-      <c r="S45">
-        <v>67.390060786486359</v>
-      </c>
-      <c r="T45">
-        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.2">
@@ -4818,51 +4557,12 @@
       <c r="B46" t="s">
         <v>11</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C46">
         <f>IF(SUMPRODUCT(--(E46:AI46&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
-      </c>
-      <c r="H46">
-        <v>71.107610250864482</v>
-      </c>
-      <c r="I46">
-        <v>80.397495895146989</v>
-      </c>
-      <c r="J46">
-        <v>81.97907665494813</v>
-      </c>
-      <c r="K46">
-        <v>85.897044557869506</v>
-      </c>
-      <c r="L46">
-        <v>84.117663131886758</v>
-      </c>
-      <c r="M46">
-        <v>78.64087048335972</v>
-      </c>
-      <c r="N46">
-        <v>86.70782189226864</v>
-      </c>
-      <c r="O46">
-        <v>83.601205293783707</v>
-      </c>
-      <c r="P46">
-        <v>80.339542554055541</v>
-      </c>
-      <c r="Q46">
-        <v>78.933328466371606</v>
-      </c>
-      <c r="R46">
-        <v>75.097231799897344</v>
-      </c>
-      <c r="S46">
-        <v>67.390060786486359</v>
-      </c>
-      <c r="T46">
-        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.2">
@@ -4889,56 +4589,17 @@
       <c r="B48" t="s">
         <v>11</v>
       </c>
-      <c r="C48" t="str">
+      <c r="C48">
         <f>IF(SUMPRODUCT(--(E48:AI48&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
-      </c>
-      <c r="H48">
-        <v>71.107610250864482</v>
-      </c>
-      <c r="I48">
-        <v>80.397495895146989</v>
-      </c>
-      <c r="J48">
-        <v>81.97907665494813</v>
-      </c>
-      <c r="K48">
-        <v>85.897044557869506</v>
-      </c>
-      <c r="L48">
-        <v>84.117663131886758</v>
-      </c>
-      <c r="M48">
-        <v>78.64087048335972</v>
-      </c>
-      <c r="N48">
-        <v>86.70782189226864</v>
-      </c>
-      <c r="O48">
-        <v>83.601205293783707</v>
-      </c>
-      <c r="P48">
-        <v>80.339542554055541</v>
-      </c>
-      <c r="Q48">
-        <v>78.933328466371606</v>
-      </c>
-      <c r="R48">
-        <v>75.097231799897344</v>
-      </c>
-      <c r="S48">
-        <v>67.390060786486359</v>
-      </c>
-      <c r="T48">
-        <v>62.74354093103689</v>
       </c>
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -5122,7 +4783,7 @@
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -5248,12 +4909,51 @@
       <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="str">
         <f>IF(SUMPRODUCT(--(E59:AI59&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
+      </c>
+      <c r="H59">
+        <v>187.2257230824689</v>
+      </c>
+      <c r="I59">
+        <v>200.7691707715197</v>
+      </c>
+      <c r="J59">
+        <v>192.68759001171856</v>
+      </c>
+      <c r="K59">
+        <v>186.99184433101937</v>
+      </c>
+      <c r="L59">
+        <v>171.99344797922433</v>
+      </c>
+      <c r="M59">
+        <v>152.58135173886251</v>
+      </c>
+      <c r="N59">
+        <v>160.45884477439802</v>
+      </c>
+      <c r="O59">
+        <v>147.67657248399411</v>
+      </c>
+      <c r="P59">
+        <v>135.66045744594447</v>
+      </c>
+      <c r="Q59">
+        <v>128.67778264473947</v>
+      </c>
+      <c r="R59">
+        <v>119.79165708899157</v>
+      </c>
+      <c r="S59">
+        <v>106.94327254684698</v>
+      </c>
+      <c r="T59">
+        <v>100.53423684674091</v>
       </c>
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.2">
@@ -5264,12 +4964,51 @@
       <c r="B60" t="s">
         <v>11</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="str">
         <f>IF(SUMPRODUCT(--(E60:AI60&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D60" t="s">
         <v>12</v>
+      </c>
+      <c r="H60">
+        <v>5166.666666666667</v>
+      </c>
+      <c r="I60">
+        <v>5623.333333333333</v>
+      </c>
+      <c r="J60">
+        <v>5493.333333333333</v>
+      </c>
+      <c r="K60">
+        <v>5457.7777777777774</v>
+      </c>
+      <c r="L60">
+        <v>5122.2222222222217</v>
+      </c>
+      <c r="M60">
+        <v>4624.4444444444443</v>
+      </c>
+      <c r="N60">
+        <v>4943.333333333333</v>
+      </c>
+      <c r="O60">
+        <v>4625.5555555555557</v>
+      </c>
+      <c r="P60">
+        <v>4320</v>
+      </c>
+      <c r="Q60">
+        <v>4152.2222222222217</v>
+      </c>
+      <c r="R60">
+        <v>3897.7777777777778</v>
+      </c>
+      <c r="S60">
+        <v>3486.6666666666665</v>
+      </c>
+      <c r="T60">
+        <v>3265.5555555555557</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.2">
@@ -5296,321 +5035,59 @@
       <c r="B62" t="s">
         <v>11</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="str">
         <f>IF(SUMPRODUCT(--(E62:AI62&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>21</v>
-      </c>
-      <c r="B64" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64">
-        <v>2000</v>
-      </c>
-      <c r="F64">
-        <v>2001</v>
-      </c>
-      <c r="G64">
-        <v>2002</v>
-      </c>
-      <c r="H64">
-        <v>2003</v>
-      </c>
-      <c r="I64">
-        <v>2004</v>
-      </c>
-      <c r="J64">
-        <v>2005</v>
-      </c>
-      <c r="K64">
-        <v>2006</v>
-      </c>
-      <c r="L64">
-        <v>2007</v>
-      </c>
-      <c r="M64">
-        <v>2008</v>
-      </c>
-      <c r="N64">
-        <v>2009</v>
-      </c>
-      <c r="O64">
-        <v>2010</v>
-      </c>
-      <c r="P64">
-        <v>2011</v>
-      </c>
-      <c r="Q64">
-        <v>2012</v>
-      </c>
-      <c r="R64">
-        <v>2013</v>
-      </c>
-      <c r="S64">
-        <v>2014</v>
-      </c>
-      <c r="T64">
-        <v>2015</v>
-      </c>
-      <c r="U64">
-        <v>2016</v>
-      </c>
-      <c r="V64">
-        <v>2017</v>
-      </c>
-      <c r="W64">
-        <v>2018</v>
-      </c>
-      <c r="X64">
-        <v>2019</v>
-      </c>
-      <c r="Y64">
-        <v>2020</v>
-      </c>
-      <c r="Z64">
-        <v>2021</v>
-      </c>
-      <c r="AA64">
-        <v>2022</v>
-      </c>
-      <c r="AB64">
-        <v>2023</v>
-      </c>
-      <c r="AC64">
-        <v>2024</v>
-      </c>
-      <c r="AD64">
-        <v>2025</v>
-      </c>
-      <c r="AE64">
-        <v>2026</v>
-      </c>
-      <c r="AF64">
-        <v>2027</v>
-      </c>
-      <c r="AG64">
-        <v>2028</v>
-      </c>
-      <c r="AH64">
-        <v>2029</v>
-      </c>
-      <c r="AI64">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A65" t="str">
-        <f>'Population Definitions'!A2</f>
-        <v>0-4</v>
-      </c>
-      <c r="B65" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65">
-        <f>IF(SUMPRODUCT(--(E65:AI65&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D65" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A66" t="str">
-        <f>'Population Definitions'!A3</f>
-        <v>5-14</v>
-      </c>
-      <c r="B66" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" t="str">
-        <f>IF(SUMPRODUCT(--(E66:AI66&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
-      </c>
-      <c r="D66" t="s">
-        <v>12</v>
-      </c>
-      <c r="H66">
-        <v>187.2257230824689</v>
-      </c>
-      <c r="I66">
-        <v>200.7691707715197</v>
-      </c>
-      <c r="J66">
-        <v>192.68759001171856</v>
-      </c>
-      <c r="K66">
-        <v>186.99184433101937</v>
-      </c>
-      <c r="L66">
-        <v>171.99344797922433</v>
-      </c>
-      <c r="M66">
-        <v>152.58135173886251</v>
-      </c>
-      <c r="N66">
-        <v>160.45884477439802</v>
-      </c>
-      <c r="O66">
-        <v>147.67657248399411</v>
-      </c>
-      <c r="P66">
-        <v>135.66045744594447</v>
-      </c>
-      <c r="Q66">
-        <v>128.67778264473947</v>
-      </c>
-      <c r="R66">
-        <v>119.79165708899157</v>
-      </c>
-      <c r="S66">
-        <v>106.94327254684698</v>
-      </c>
-      <c r="T66">
-        <v>100.53423684674091</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A67" t="str">
-        <f>'Population Definitions'!A4</f>
-        <v>15-64</v>
-      </c>
-      <c r="B67" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" t="str">
-        <f>IF(SUMPRODUCT(--(E67:AI67&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
-      </c>
-      <c r="D67" t="s">
-        <v>12</v>
-      </c>
-      <c r="H67">
-        <v>5166.666666666667</v>
-      </c>
-      <c r="I67">
-        <v>5623.333333333333</v>
-      </c>
-      <c r="J67">
-        <v>5493.333333333333</v>
-      </c>
-      <c r="K67">
-        <v>5457.7777777777774</v>
-      </c>
-      <c r="L67">
-        <v>5122.2222222222217</v>
-      </c>
-      <c r="M67">
-        <v>4624.4444444444443</v>
-      </c>
-      <c r="N67">
-        <v>4943.333333333333</v>
-      </c>
-      <c r="O67">
-        <v>4625.5555555555557</v>
-      </c>
-      <c r="P67">
-        <v>4320</v>
-      </c>
-      <c r="Q67">
-        <v>4152.2222222222217</v>
-      </c>
-      <c r="R67">
-        <v>3897.7777777777778</v>
-      </c>
-      <c r="S67">
-        <v>3486.6666666666665</v>
-      </c>
-      <c r="T67">
-        <v>3265.5555555555557</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A68" t="str">
-        <f>'Population Definitions'!A5</f>
-        <v>65+</v>
-      </c>
-      <c r="B68" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68">
-        <f>IF(SUMPRODUCT(--(E68:AI68&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
-      </c>
-      <c r="D68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A69" t="str">
-        <f>'Population Definitions'!A6</f>
-        <v>Prisoners</v>
-      </c>
-      <c r="B69" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" t="str">
-        <f>IF(SUMPRODUCT(--(E69:AI69&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>N.A.</v>
-      </c>
-      <c r="D69" t="s">
-        <v>12</v>
-      </c>
-      <c r="H69">
+      <c r="H62">
         <v>456.66666666666663</v>
       </c>
-      <c r="I69">
+      <c r="I62">
         <v>413.33333333333331</v>
       </c>
-      <c r="J69">
+      <c r="J62">
         <v>404.44444444444446</v>
       </c>
-      <c r="K69">
+      <c r="K62">
         <v>255.55555555555554</v>
       </c>
-      <c r="L69">
+      <c r="L62">
         <v>291.11111111111109</v>
       </c>
-      <c r="M69">
+      <c r="M62">
         <v>270</v>
       </c>
-      <c r="N69">
+      <c r="N62">
         <v>182.22222222222223</v>
       </c>
-      <c r="O69">
+      <c r="O62">
         <v>167.77777777777777</v>
       </c>
-      <c r="P69">
+      <c r="P62">
         <v>154.44444444444443</v>
       </c>
-      <c r="Q69">
+      <c r="Q62">
         <v>176.66666666666666</v>
       </c>
-      <c r="R69">
+      <c r="R62">
         <v>117.77777777777777</v>
       </c>
-      <c r="S69">
+      <c r="S62">
         <v>116.66666666666666</v>
       </c>
-      <c r="T69">
+      <c r="T62">
         <v>92.222222222222214</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B65:B69 B58:B62 B51:B55 B44:B48 B9:B13 B2:B6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B58:B62 B51:B55 B44:B48 B37:B41 B2:B6">
       <formula1>"Number"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B37:B41 B30:B34 B23:B27 B16:B20">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B30:B34 B23:B27 B16:B20 B9:B13">
       <formula1>"Fraction"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5622,7 +5099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI524"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="C233" sqref="C233:C237"/>
     </sheetView>
   </sheetViews>

</xml_diff>